<commit_message>
added allure report configuration V1
</commit_message>
<xml_diff>
--- a/target/generated-sources/usersData.xlsx
+++ b/target/generated-sources/usersData.xlsx
@@ -14,304 +14,304 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
-    <t>Afet Mayhoş</t>
-  </si>
-  <si>
-    <t>Samantha Franklin</t>
-  </si>
-  <si>
-    <t>Melvin Richardson</t>
-  </si>
-  <si>
-    <t>Marina Navarro</t>
-  </si>
-  <si>
-    <t>Guiliano Verschure</t>
-  </si>
-  <si>
-    <t>Thorbjørn Nordal</t>
-  </si>
-  <si>
-    <t>Chloe Thompson</t>
-  </si>
-  <si>
-    <t>Isabelle Skullerud</t>
-  </si>
-  <si>
-    <t>Harrison Wang</t>
-  </si>
-  <si>
-    <t>Ezio Morel</t>
-  </si>
-  <si>
-    <t>Calvin Brown</t>
-  </si>
-  <si>
-    <t>Ruby Cooper</t>
-  </si>
-  <si>
-    <t>آنیتا محمدخان</t>
-  </si>
-  <si>
-    <t>Milena Kalinowski</t>
-  </si>
-  <si>
-    <t>Mikael Spanjaard</t>
-  </si>
-  <si>
-    <t>پریا پارسا</t>
-  </si>
-  <si>
-    <t>Noémie Wilson</t>
-  </si>
-  <si>
-    <t>Loan Chevalier</t>
-  </si>
-  <si>
-    <t>Andrea Pedersen</t>
-  </si>
-  <si>
-    <t>Samantha Roberts</t>
-  </si>
-  <si>
-    <t>Doris Castro</t>
-  </si>
-  <si>
-    <t>Kévim Moura</t>
-  </si>
-  <si>
-    <t>علیرضا گلشن</t>
-  </si>
-  <si>
-    <t>Victor Chan</t>
-  </si>
-  <si>
-    <t>Dolores Herrera</t>
-  </si>
-  <si>
-    <t>Heleen De Pee</t>
-  </si>
-  <si>
-    <t>Aapo Haapala</t>
-  </si>
-  <si>
-    <t>Oliver Harju</t>
-  </si>
-  <si>
-    <t>Mackenzie Clarke</t>
-  </si>
-  <si>
-    <t>Eduardo Reed</t>
-  </si>
-  <si>
-    <t>Estéban Olivier</t>
-  </si>
-  <si>
-    <t>Polle Zoontjens</t>
-  </si>
-  <si>
-    <t>Martin Heinrich</t>
-  </si>
-  <si>
-    <t>Koray Taşçı</t>
-  </si>
-  <si>
-    <t>Arnaud Roy</t>
-  </si>
-  <si>
-    <t>آوینا پارسا</t>
-  </si>
-  <si>
-    <t>Anielo Mendes</t>
-  </si>
-  <si>
-    <t>Victoire Rodriguez</t>
-  </si>
-  <si>
-    <t>Maxime Harcourt</t>
-  </si>
-  <si>
-    <t>Iina Ylitalo</t>
-  </si>
-  <si>
-    <t>Matusalém Gomes</t>
-  </si>
-  <si>
-    <t>Jocelaine Teixeira</t>
-  </si>
-  <si>
-    <t>Justin Grewal</t>
-  </si>
-  <si>
-    <t>Aapo Kokko</t>
-  </si>
-  <si>
-    <t>Luis Rolland</t>
-  </si>
-  <si>
-    <t>Zoe Moore</t>
-  </si>
-  <si>
-    <t>Seth Van Apeldoorn</t>
-  </si>
-  <si>
-    <t>Sylvio Hirschmann</t>
-  </si>
-  <si>
-    <t>Sümeyye Den Exter</t>
-  </si>
-  <si>
-    <t>Maeva Bouchard</t>
-  </si>
-  <si>
-    <t>Abigail Banks</t>
-  </si>
-  <si>
-    <t>Paulina Underhaug</t>
-  </si>
-  <si>
-    <t>Amy Powell</t>
-  </si>
-  <si>
-    <t>Deniz Poçan</t>
-  </si>
-  <si>
-    <t>النا کامروا</t>
-  </si>
-  <si>
-    <t>Hailey Terry</t>
-  </si>
-  <si>
-    <t>Natascha Dupuis</t>
-  </si>
-  <si>
-    <t>Christine Mcdonalid</t>
-  </si>
-  <si>
-    <t>Harper Chu</t>
-  </si>
-  <si>
-    <t>Oğuzhan Sepetçi</t>
-  </si>
-  <si>
-    <t>سورنا علیزاده</t>
-  </si>
-  <si>
-    <t>Michaela Woertman</t>
-  </si>
-  <si>
-    <t>Douglas Armstrong</t>
-  </si>
-  <si>
-    <t>Herlander Martins</t>
-  </si>
-  <si>
-    <t>Lillian Thomas</t>
-  </si>
-  <si>
-    <t>Kerim Bademci</t>
-  </si>
-  <si>
-    <t>Herberto da Mota</t>
-  </si>
-  <si>
-    <t>Yedda Duarte</t>
-  </si>
-  <si>
-    <t>Line Lemoine</t>
-  </si>
-  <si>
-    <t>Raffaele Lacroix</t>
-  </si>
-  <si>
-    <t>Sílvio da Paz</t>
-  </si>
-  <si>
-    <t>Hung Klopper</t>
-  </si>
-  <si>
-    <t>Nurdan Kumcuoğlu</t>
-  </si>
-  <si>
-    <t>Elisa Vazquez</t>
-  </si>
-  <si>
-    <t>Lotti Storz</t>
-  </si>
-  <si>
-    <t>سورنا سالاری</t>
-  </si>
-  <si>
-    <t>Lotte Pettersen</t>
-  </si>
-  <si>
-    <t>Aapo Aho</t>
-  </si>
-  <si>
-    <t>Mads Petersen</t>
-  </si>
-  <si>
-    <t>Joel Peltonen</t>
-  </si>
-  <si>
-    <t>Marceau Robin</t>
-  </si>
-  <si>
-    <t>Próspero Mendes</t>
-  </si>
-  <si>
-    <t>Walda Nunes</t>
-  </si>
-  <si>
-    <t>Laura Larsen</t>
-  </si>
-  <si>
-    <t>Christer Sommerstad</t>
-  </si>
-  <si>
-    <t>Elias Kujala</t>
-  </si>
-  <si>
-    <t>هستی علیزاده</t>
-  </si>
-  <si>
-    <t>Brandy Davidson</t>
-  </si>
-  <si>
-    <t>Frederique Gooijer</t>
-  </si>
-  <si>
-    <t>Nalan Akışık</t>
-  </si>
-  <si>
-    <t>Elvi Ivens</t>
-  </si>
-  <si>
-    <t>Bradley Stanley</t>
-  </si>
-  <si>
-    <t>Alfred Pedersen</t>
-  </si>
-  <si>
-    <t>Evelyn Hart</t>
-  </si>
-  <si>
-    <t>Eli Horton</t>
-  </si>
-  <si>
-    <t>Bradley Young</t>
-  </si>
-  <si>
-    <t>Cecilie Larsen</t>
-  </si>
-  <si>
-    <t>Jonathan Martin</t>
-  </si>
-  <si>
-    <t>Vitus Glöckner</t>
-  </si>
-  <si>
-    <t>Marc Muñoz</t>
+    <t>Franklim Moraes</t>
+  </si>
+  <si>
+    <t>Ana Lecomte</t>
+  </si>
+  <si>
+    <t>Leanne Scott</t>
+  </si>
+  <si>
+    <t>Irina Girard</t>
+  </si>
+  <si>
+    <t>بردیا سهيلي راد</t>
+  </si>
+  <si>
+    <t>Alexander Claire</t>
+  </si>
+  <si>
+    <t>Catalina Ribeiro</t>
+  </si>
+  <si>
+    <t>Hugo Edwards</t>
+  </si>
+  <si>
+    <t>دینا جعفری</t>
+  </si>
+  <si>
+    <t>Åsa Kristensen</t>
+  </si>
+  <si>
+    <t>Emma Johnson</t>
+  </si>
+  <si>
+    <t>Frederick Sutton</t>
+  </si>
+  <si>
+    <t>Leonício Rocha</t>
+  </si>
+  <si>
+    <t>Judith Edwards</t>
+  </si>
+  <si>
+    <t>Sofia Poulsen</t>
+  </si>
+  <si>
+    <t>Toby Zhang</t>
+  </si>
+  <si>
+    <t>Loreto Pires</t>
+  </si>
+  <si>
+    <t>Liva Nielsen</t>
+  </si>
+  <si>
+    <t>Luise Oliveira</t>
+  </si>
+  <si>
+    <t>Benito Jimenez</t>
+  </si>
+  <si>
+    <t>رها محمدخان</t>
+  </si>
+  <si>
+    <t>Deniz Çetin</t>
+  </si>
+  <si>
+    <t>Carmen Henderson</t>
+  </si>
+  <si>
+    <t>Joanna Neher</t>
+  </si>
+  <si>
+    <t>Alex Graham</t>
+  </si>
+  <si>
+    <t>سارا نكو نظر</t>
+  </si>
+  <si>
+    <t>Toni Jennings</t>
+  </si>
+  <si>
+    <t>Roberto Ortega</t>
+  </si>
+  <si>
+    <t>Susanna Riley</t>
+  </si>
+  <si>
+    <t>آریا سهيلي راد</t>
+  </si>
+  <si>
+    <t>Yasemin Baturalp</t>
+  </si>
+  <si>
+    <t>Gonca Çapanoğlu</t>
+  </si>
+  <si>
+    <t>Timen Reijers</t>
+  </si>
+  <si>
+    <t>Vicenta Vargas</t>
+  </si>
+  <si>
+    <t>Samuel Makinen</t>
+  </si>
+  <si>
+    <t>Kirstin Eismann</t>
+  </si>
+  <si>
+    <t>Raphaël Bourgeois</t>
+  </si>
+  <si>
+    <t>Adeli Ramos</t>
+  </si>
+  <si>
+    <t>Oswald Schreyer</t>
+  </si>
+  <si>
+    <t>Arsen Janga</t>
+  </si>
+  <si>
+    <t>Sander Mortensen</t>
+  </si>
+  <si>
+    <t>Kenneth Taylor</t>
+  </si>
+  <si>
+    <t>Lorraine Jimenez</t>
+  </si>
+  <si>
+    <t>Cassandra Wells</t>
+  </si>
+  <si>
+    <t>Medina Rohde</t>
+  </si>
+  <si>
+    <t>Alex Groven</t>
+  </si>
+  <si>
+    <t>Miguel Lopez</t>
+  </si>
+  <si>
+    <t>Marvin Løland</t>
+  </si>
+  <si>
+    <t>Leah Porter</t>
+  </si>
+  <si>
+    <t>Niilo Ruona</t>
+  </si>
+  <si>
+    <t>Gema Vidal</t>
+  </si>
+  <si>
+    <t>Miriam Steinhauer</t>
+  </si>
+  <si>
+    <t>Jorgo Paling</t>
+  </si>
+  <si>
+    <t>Hanspeter Gonzalez</t>
+  </si>
+  <si>
+    <t>Misja Van Beijnum</t>
+  </si>
+  <si>
+    <t>Dané Binda</t>
+  </si>
+  <si>
+    <t>Enise Van Eldijk</t>
+  </si>
+  <si>
+    <t>Yvone Almeida</t>
+  </si>
+  <si>
+    <t>Brian Nekstad</t>
+  </si>
+  <si>
+    <t>Lisa Hayes</t>
+  </si>
+  <si>
+    <t>Eeli Hietala</t>
+  </si>
+  <si>
+    <t>علی رضا گلشن</t>
+  </si>
+  <si>
+    <t>Tanneke Van Gorkum</t>
+  </si>
+  <si>
+    <t>Gilbert Hudson</t>
+  </si>
+  <si>
+    <t>Alberte Kristensen</t>
+  </si>
+  <si>
+    <t>Willard Howard</t>
+  </si>
+  <si>
+    <t>Robby Haverkate</t>
+  </si>
+  <si>
+    <t>مانی حیدری</t>
+  </si>
+  <si>
+    <t>Fatin Hoogendijk</t>
+  </si>
+  <si>
+    <t>Maud Ditlefsen</t>
+  </si>
+  <si>
+    <t>Miro Takala</t>
+  </si>
+  <si>
+    <t>Leah Edwards</t>
+  </si>
+  <si>
+    <t>Aubri Novaes</t>
+  </si>
+  <si>
+    <t>Victoria Christiansen</t>
+  </si>
+  <si>
+    <t>Liam Jones</t>
+  </si>
+  <si>
+    <t>Kate Neal</t>
+  </si>
+  <si>
+    <t>Beatrice Thompson</t>
+  </si>
+  <si>
+    <t>Joona Hakola</t>
+  </si>
+  <si>
+    <t>Jeanne Park</t>
+  </si>
+  <si>
+    <t>Kayra Vaassen</t>
+  </si>
+  <si>
+    <t>Hanna Martinez</t>
+  </si>
+  <si>
+    <t>Gabino Viana</t>
+  </si>
+  <si>
+    <t>Ella Mortensen</t>
+  </si>
+  <si>
+    <t>Ylona Burema</t>
+  </si>
+  <si>
+    <t>Rosalinde Bos</t>
+  </si>
+  <si>
+    <t>Wishal Thoma</t>
+  </si>
+  <si>
+    <t>Richard Helle</t>
+  </si>
+  <si>
+    <t>Mikkel Rasmussen</t>
+  </si>
+  <si>
+    <t>Erin Price</t>
+  </si>
+  <si>
+    <t>Lisa Murray</t>
+  </si>
+  <si>
+    <t>Maëlys Francois</t>
+  </si>
+  <si>
+    <t>Adem Erbulak</t>
+  </si>
+  <si>
+    <t>Aino Rajala</t>
+  </si>
+  <si>
+    <t>Raphaël Rey</t>
+  </si>
+  <si>
+    <t>Patricia Marin</t>
+  </si>
+  <si>
+    <t>Cecilia Brede</t>
+  </si>
+  <si>
+    <t>Jessica Smith</t>
+  </si>
+  <si>
+    <t>Encarnacion Campos</t>
+  </si>
+  <si>
+    <t>Valdemar Jensen</t>
+  </si>
+  <si>
+    <t>Efe Erçetin</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
configuration for cucumber report
</commit_message>
<xml_diff>
--- a/target/generated-sources/usersData.xlsx
+++ b/target/generated-sources/usersData.xlsx
@@ -14,304 +14,304 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
-    <t>Afet Mayhoş</t>
-  </si>
-  <si>
-    <t>Samantha Franklin</t>
-  </si>
-  <si>
-    <t>Melvin Richardson</t>
-  </si>
-  <si>
-    <t>Marina Navarro</t>
-  </si>
-  <si>
-    <t>Guiliano Verschure</t>
-  </si>
-  <si>
-    <t>Thorbjørn Nordal</t>
-  </si>
-  <si>
-    <t>Chloe Thompson</t>
-  </si>
-  <si>
-    <t>Isabelle Skullerud</t>
-  </si>
-  <si>
-    <t>Harrison Wang</t>
-  </si>
-  <si>
-    <t>Ezio Morel</t>
-  </si>
-  <si>
-    <t>Calvin Brown</t>
-  </si>
-  <si>
-    <t>Ruby Cooper</t>
-  </si>
-  <si>
-    <t>آنیتا محمدخان</t>
-  </si>
-  <si>
-    <t>Milena Kalinowski</t>
-  </si>
-  <si>
-    <t>Mikael Spanjaard</t>
-  </si>
-  <si>
-    <t>پریا پارسا</t>
-  </si>
-  <si>
-    <t>Noémie Wilson</t>
-  </si>
-  <si>
-    <t>Loan Chevalier</t>
-  </si>
-  <si>
-    <t>Andrea Pedersen</t>
-  </si>
-  <si>
-    <t>Samantha Roberts</t>
-  </si>
-  <si>
-    <t>Doris Castro</t>
-  </si>
-  <si>
-    <t>Kévim Moura</t>
-  </si>
-  <si>
-    <t>علیرضا گلشن</t>
-  </si>
-  <si>
-    <t>Victor Chan</t>
-  </si>
-  <si>
-    <t>Dolores Herrera</t>
-  </si>
-  <si>
-    <t>Heleen De Pee</t>
-  </si>
-  <si>
-    <t>Aapo Haapala</t>
-  </si>
-  <si>
-    <t>Oliver Harju</t>
-  </si>
-  <si>
-    <t>Mackenzie Clarke</t>
-  </si>
-  <si>
-    <t>Eduardo Reed</t>
-  </si>
-  <si>
-    <t>Estéban Olivier</t>
-  </si>
-  <si>
-    <t>Polle Zoontjens</t>
-  </si>
-  <si>
-    <t>Martin Heinrich</t>
-  </si>
-  <si>
-    <t>Koray Taşçı</t>
-  </si>
-  <si>
-    <t>Arnaud Roy</t>
-  </si>
-  <si>
-    <t>آوینا پارسا</t>
-  </si>
-  <si>
-    <t>Anielo Mendes</t>
-  </si>
-  <si>
-    <t>Victoire Rodriguez</t>
-  </si>
-  <si>
-    <t>Maxime Harcourt</t>
-  </si>
-  <si>
-    <t>Iina Ylitalo</t>
-  </si>
-  <si>
-    <t>Matusalém Gomes</t>
-  </si>
-  <si>
-    <t>Jocelaine Teixeira</t>
-  </si>
-  <si>
-    <t>Justin Grewal</t>
-  </si>
-  <si>
-    <t>Aapo Kokko</t>
-  </si>
-  <si>
-    <t>Luis Rolland</t>
-  </si>
-  <si>
-    <t>Zoe Moore</t>
-  </si>
-  <si>
-    <t>Seth Van Apeldoorn</t>
-  </si>
-  <si>
-    <t>Sylvio Hirschmann</t>
-  </si>
-  <si>
-    <t>Sümeyye Den Exter</t>
-  </si>
-  <si>
-    <t>Maeva Bouchard</t>
-  </si>
-  <si>
-    <t>Abigail Banks</t>
-  </si>
-  <si>
-    <t>Paulina Underhaug</t>
-  </si>
-  <si>
-    <t>Amy Powell</t>
-  </si>
-  <si>
-    <t>Deniz Poçan</t>
-  </si>
-  <si>
-    <t>النا کامروا</t>
-  </si>
-  <si>
-    <t>Hailey Terry</t>
-  </si>
-  <si>
-    <t>Natascha Dupuis</t>
-  </si>
-  <si>
-    <t>Christine Mcdonalid</t>
-  </si>
-  <si>
-    <t>Harper Chu</t>
-  </si>
-  <si>
-    <t>Oğuzhan Sepetçi</t>
-  </si>
-  <si>
-    <t>سورنا علیزاده</t>
-  </si>
-  <si>
-    <t>Michaela Woertman</t>
-  </si>
-  <si>
-    <t>Douglas Armstrong</t>
-  </si>
-  <si>
-    <t>Herlander Martins</t>
-  </si>
-  <si>
-    <t>Lillian Thomas</t>
-  </si>
-  <si>
-    <t>Kerim Bademci</t>
-  </si>
-  <si>
-    <t>Herberto da Mota</t>
-  </si>
-  <si>
-    <t>Yedda Duarte</t>
-  </si>
-  <si>
-    <t>Line Lemoine</t>
-  </si>
-  <si>
-    <t>Raffaele Lacroix</t>
-  </si>
-  <si>
-    <t>Sílvio da Paz</t>
-  </si>
-  <si>
-    <t>Hung Klopper</t>
-  </si>
-  <si>
-    <t>Nurdan Kumcuoğlu</t>
-  </si>
-  <si>
-    <t>Elisa Vazquez</t>
-  </si>
-  <si>
-    <t>Lotti Storz</t>
-  </si>
-  <si>
-    <t>سورنا سالاری</t>
-  </si>
-  <si>
-    <t>Lotte Pettersen</t>
-  </si>
-  <si>
-    <t>Aapo Aho</t>
-  </si>
-  <si>
-    <t>Mads Petersen</t>
-  </si>
-  <si>
-    <t>Joel Peltonen</t>
-  </si>
-  <si>
-    <t>Marceau Robin</t>
-  </si>
-  <si>
-    <t>Próspero Mendes</t>
-  </si>
-  <si>
-    <t>Walda Nunes</t>
-  </si>
-  <si>
-    <t>Laura Larsen</t>
-  </si>
-  <si>
-    <t>Christer Sommerstad</t>
-  </si>
-  <si>
-    <t>Elias Kujala</t>
-  </si>
-  <si>
-    <t>هستی علیزاده</t>
-  </si>
-  <si>
-    <t>Brandy Davidson</t>
-  </si>
-  <si>
-    <t>Frederique Gooijer</t>
-  </si>
-  <si>
-    <t>Nalan Akışık</t>
-  </si>
-  <si>
-    <t>Elvi Ivens</t>
-  </si>
-  <si>
-    <t>Bradley Stanley</t>
-  </si>
-  <si>
-    <t>Alfred Pedersen</t>
-  </si>
-  <si>
-    <t>Evelyn Hart</t>
-  </si>
-  <si>
-    <t>Eli Horton</t>
-  </si>
-  <si>
-    <t>Bradley Young</t>
-  </si>
-  <si>
-    <t>Cecilie Larsen</t>
-  </si>
-  <si>
-    <t>Jonathan Martin</t>
-  </si>
-  <si>
-    <t>Vitus Glöckner</t>
-  </si>
-  <si>
-    <t>Marc Muñoz</t>
+    <t>Isabell Benecke</t>
+  </si>
+  <si>
+    <t>Peyton Turner</t>
+  </si>
+  <si>
+    <t>Maëline Moreau</t>
+  </si>
+  <si>
+    <t>Tiago Roger</t>
+  </si>
+  <si>
+    <t>Dioclécio Aragão</t>
+  </si>
+  <si>
+    <t>Carina Warholm</t>
+  </si>
+  <si>
+    <t>Dorina Bielefeld</t>
+  </si>
+  <si>
+    <t>بیتا قاسمی</t>
+  </si>
+  <si>
+    <t>Jasmin Raab</t>
+  </si>
+  <si>
+    <t>Flora Renaud</t>
+  </si>
+  <si>
+    <t>Carmen Torres</t>
+  </si>
+  <si>
+    <t>Ivanilda Teixeira</t>
+  </si>
+  <si>
+    <t>Ülkü Kunt</t>
+  </si>
+  <si>
+    <t>Teo Hammervold</t>
+  </si>
+  <si>
+    <t>Roope Tikkanen</t>
+  </si>
+  <si>
+    <t>Roope Ylitalo</t>
+  </si>
+  <si>
+    <t>Wanner Campos</t>
+  </si>
+  <si>
+    <t>Luiziane Rezende</t>
+  </si>
+  <si>
+    <t>Patricia Mcdonalid</t>
+  </si>
+  <si>
+    <t>كيان جعفری</t>
+  </si>
+  <si>
+    <t>Etienne Abraham</t>
+  </si>
+  <si>
+    <t>Karianne Aune</t>
+  </si>
+  <si>
+    <t>Adam Blanchard</t>
+  </si>
+  <si>
+    <t>Ewen Fernandez</t>
+  </si>
+  <si>
+    <t>Suzanna Ramirez</t>
+  </si>
+  <si>
+    <t>Kasper Korhonen</t>
+  </si>
+  <si>
+    <t>Timian Trøen</t>
+  </si>
+  <si>
+    <t>Mia Jean-Baptiste</t>
+  </si>
+  <si>
+    <t>یسنا حسینی</t>
+  </si>
+  <si>
+    <t>Carlos Pena</t>
+  </si>
+  <si>
+    <t>Barry Reid</t>
+  </si>
+  <si>
+    <t>Lilli Jordan</t>
+  </si>
+  <si>
+    <t>Lester Morrison</t>
+  </si>
+  <si>
+    <t>Andy Hansen</t>
+  </si>
+  <si>
+    <t>Väinö Ruona</t>
+  </si>
+  <si>
+    <t>Katharina Laterveer</t>
+  </si>
+  <si>
+    <t>Ernest Taylor</t>
+  </si>
+  <si>
+    <t>Ella Harcourt</t>
+  </si>
+  <si>
+    <t>Cindy Chavez</t>
+  </si>
+  <si>
+    <t>Alejandra Reyes</t>
+  </si>
+  <si>
+    <t>Daniel French</t>
+  </si>
+  <si>
+    <t>Arlo Walker</t>
+  </si>
+  <si>
+    <t>Carl Riley</t>
+  </si>
+  <si>
+    <t>Mechelina Morssink</t>
+  </si>
+  <si>
+    <t>Eeli Neva</t>
+  </si>
+  <si>
+    <t>Süreyya Van der Kemp</t>
+  </si>
+  <si>
+    <t>Nihal Balaban</t>
+  </si>
+  <si>
+    <t>Maritza Verwijmeren</t>
+  </si>
+  <si>
+    <t>Delores Powell</t>
+  </si>
+  <si>
+    <t>Marvin Perry</t>
+  </si>
+  <si>
+    <t>Tino Schmieder</t>
+  </si>
+  <si>
+    <t>Jordan Bell</t>
+  </si>
+  <si>
+    <t>Florent Meyer</t>
+  </si>
+  <si>
+    <t>Fatih Akan</t>
+  </si>
+  <si>
+    <t>Roberto Cox</t>
+  </si>
+  <si>
+    <t>Todd Banks</t>
+  </si>
+  <si>
+    <t>Reginald Carpenter</t>
+  </si>
+  <si>
+    <t>Wallace Mccoy</t>
+  </si>
+  <si>
+    <t>Tomas Martin</t>
+  </si>
+  <si>
+    <t>Marita Hilmer</t>
+  </si>
+  <si>
+    <t>Jeremiah Chambers</t>
+  </si>
+  <si>
+    <t>David Martin</t>
+  </si>
+  <si>
+    <t>Theo Smith</t>
+  </si>
+  <si>
+    <t>Arvid Magnussen</t>
+  </si>
+  <si>
+    <t>Anders Svee</t>
+  </si>
+  <si>
+    <t>Noémie White</t>
+  </si>
+  <si>
+    <t>Gianna Lecomte</t>
+  </si>
+  <si>
+    <t>Bartje Keur</t>
+  </si>
+  <si>
+    <t>Nieves Ibañez</t>
+  </si>
+  <si>
+    <t>Carolina Caballero</t>
+  </si>
+  <si>
+    <t>Ivaldo Nunes</t>
+  </si>
+  <si>
+    <t>Rosalyn Craig</t>
+  </si>
+  <si>
+    <t>Hilda Warren</t>
+  </si>
+  <si>
+    <t>Tyler Moore</t>
+  </si>
+  <si>
+    <t>Elizabeth Novak</t>
+  </si>
+  <si>
+    <t>Terrence Wheeler</t>
+  </si>
+  <si>
+    <t>Gabija Telle</t>
+  </si>
+  <si>
+    <t>Emilie Laurent</t>
+  </si>
+  <si>
+    <t>Gilbert Schöner</t>
+  </si>
+  <si>
+    <t>Daniel Carlson</t>
+  </si>
+  <si>
+    <t>Ella Wong</t>
+  </si>
+  <si>
+    <t>Noah Nielsen</t>
+  </si>
+  <si>
+    <t>Rose Li</t>
+  </si>
+  <si>
+    <t>Isabella Pierce</t>
+  </si>
+  <si>
+    <t>Abigail Patel</t>
+  </si>
+  <si>
+    <t>Hélèna Le Gall</t>
+  </si>
+  <si>
+    <t>Gauthier Perez</t>
+  </si>
+  <si>
+    <t>Khadija Skullerud</t>
+  </si>
+  <si>
+    <t>Emily Ross</t>
+  </si>
+  <si>
+    <t>Pihla Koskela</t>
+  </si>
+  <si>
+    <t>Aubrey Thompson</t>
+  </si>
+  <si>
+    <t>Siegrid Michl</t>
+  </si>
+  <si>
+    <t>پرهام سالاری</t>
+  </si>
+  <si>
+    <t>Jerusa Cavalcanti</t>
+  </si>
+  <si>
+    <t>Amelia Wilson</t>
+  </si>
+  <si>
+    <t>Rachel West</t>
+  </si>
+  <si>
+    <t>Nalan Kurutluoğlu</t>
+  </si>
+  <si>
+    <t>Earl Boyd</t>
+  </si>
+  <si>
+    <t>Maurice Reid</t>
+  </si>
+  <si>
+    <t>Courtney Johnson</t>
   </si>
 </sst>
 </file>

</xml_diff>